<commit_message>
TC002 Test Case and wait utils
</commit_message>
<xml_diff>
--- a/testData/Login_TestData.xlsx
+++ b/testData/Login_TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2403730\eclipse-workspace\Hackathon\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2403730\eclipse-workspace\FindingHospitals\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1914B089-80F0-437C-A239-0EC575183BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979929B4-355B-4C1D-BB13-1705510C5D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DB61F18C-A548-43C5-B09F-3FBF5DCB0077}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC004" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>